<commit_message>
Documentación - Revision SQA
Se realiza revisión SQA sobre el documento clave relacionados al plan de riesgos. Se actualiza el artefacto de trabajo para revisiones SQA.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\03-Construccion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93475CB-2233-4C38-ACD9-0F3570A4E3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1585EC-719A-402E-A682-B2AC26D2CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 Descripción:
 Nivel de gravedad:
 Ubicación:
-Si se realizó la misma revision a distintos productos ingrese la palabra "Repetido"
+Si se realizó la misma revisión a distintos productos ingrese la palabra "Repetido"
 </t>
         </r>
       </text>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="113">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -709,9 +709,6 @@
     <t>No existe mitigación</t>
   </si>
   <si>
-    <t>No se realiza re-evalación</t>
-  </si>
-  <si>
     <t>No se realiza revisión-control</t>
   </si>
   <si>
@@ -872,15 +869,6 @@
   </si>
   <si>
     <t>Elaboración 1</t>
-  </si>
-  <si>
-    <t>Construción 3</t>
-  </si>
-  <si>
-    <t>Construción 1</t>
-  </si>
-  <si>
-    <t>Construción 2</t>
   </si>
   <si>
     <t>Elaboracion iteracion 1</t>
@@ -1033,6 +1021,280 @@
   </si>
   <si>
     <t>Plan de Riesgos</t>
+  </si>
+  <si>
+    <t>Índice</t>
+  </si>
+  <si>
+    <t>No se realiza reevaluación</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en el formato de nomenclatura de nombres definido por el grupo de desarrollo OSLO.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: No se encontraron errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: No se encontraron errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\C106-OSLO - Identificación, Evaluación y análisis de riesgos - Anexo II 27-10-2024.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Referencia de índice desactualizado.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1896,7 +2158,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -1912,13 +2174,13 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1937,7 +2199,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L2">
         <f>COUNTIF(A2:A3,"*")</f>
@@ -1961,7 +2223,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L3">
         <f>COUNTIF(A4:A11,"*")</f>
@@ -1982,7 +2244,7 @@
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1999,7 +2261,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2016,7 +2278,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2033,7 +2295,7 @@
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2222,12 +2484,12 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -2237,7 +2499,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -2247,12 +2509,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -2333,7 +2595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7F18F4-1A82-4DA7-BAA1-7D801E9E7A78}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2345,7 +2607,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2355,18 +2617,18 @@
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2392,7 +2654,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
@@ -2472,7 +2734,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -2488,18 +2750,18 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2512,7 +2774,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="15"/>
       <c r="K2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L2">
         <f>COUNTIF(A2:A30,"*")</f>
@@ -2535,7 +2797,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="13"/>
       <c r="K3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2550,7 +2812,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="K4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2565,7 +2827,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="K5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2580,7 +2842,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2766,17 +3028,17 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -2884,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -2900,13 +3162,13 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3157,12 +3419,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
@@ -3267,7 +3529,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -3283,13 +3545,13 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3540,7 +3802,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -3650,7 +3912,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -3666,13 +3928,13 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3923,7 +4185,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4000,20 +4262,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="6" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="99.140625" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
@@ -4033,7 +4296,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -4049,31 +4312,45 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F2" s="16">
+        <v>45593</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L2">
         <f>COUNTIF(A2,"*")</f>
@@ -4083,52 +4360,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F3" s="17">
+        <v>45593</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="K3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3">
         <f>COUNTIF(A3:A6,"*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="12">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F4" s="17">
+        <v>45593</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="K4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F5" s="17">
+        <v>45593</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>109</v>
+      </c>
       <c r="K5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -4143,7 +4472,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="K6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4158,7 +4487,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="K7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4312,12 +4641,12 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -4327,79 +4656,84 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="6">
+  <dataValidations xWindow="732" yWindow="453" count="6">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F2:F20" xr:uid="{00000000-0002-0000-0500-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otras opciones de resultado." promptTitle="Estado" prompt="¿Fue resuelto?" sqref="G2:G20" xr:uid="{00000000-0002-0000-0500-000001000000}">
-      <formula1>$A$61:$A$63</formula1>
+      <formula1>$A$62:$A$64</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="D2:D20" xr:uid="{00000000-0002-0000-0500-000002000000}">
-      <formula1>$A$58:$A$59</formula1>
+      <formula1>$A$59:$A$60</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C2:C20" xr:uid="{00000000-0002-0000-0500-000003000000}">
-      <formula1>$A$50:$A$56</formula1>
+      <formula1>$A$50:$A$57</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Responsable" prompt="¿Que integrante del equipo de desarrollo realizo la revisión?" sqref="H2:H20" xr:uid="{00000000-0002-0000-0500-000004000000}">
-      <formula1>$A$65:$A$68</formula1>
+      <formula1>$A$66:$A$69</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" showDropDown="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="E2:E20" xr:uid="{00000000-0002-0000-0500-000005000000}"/>
   </dataValidations>
@@ -4443,7 +4777,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -4459,13 +4793,13 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4691,32 +5025,32 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4796,7 +5130,7 @@
   <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,7 +5169,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -4851,14 +5185,14 @@
       </c>
       <c r="J1" s="23"/>
       <c r="K1" s="49" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
       <c r="N1" s="50"/>
       <c r="O1" s="51"/>
       <c r="P1" s="49" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="Q1" s="50"/>
       <c r="R1" s="50"/>
@@ -4867,7 +5201,7 @@
     </row>
     <row r="2" spans="1:20" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4891,43 +5225,43 @@
         <v>18</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="P2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="25" t="s">
+      <c r="S2" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="T2" s="25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -4951,11 +5285,11 @@
         <v>18</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" s="31">
         <f>COUNTIF($A$2:$A$80, "*Estudio e Implementación UARGFLOW*")</f>
@@ -4974,7 +5308,7 @@
         <v>17</v>
       </c>
       <c r="P3" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q3" s="31">
         <f>COUNTIF($A$2:$A$80, "*Prototipo*")</f>
@@ -5005,7 +5339,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L4" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de estimación*")</f>
@@ -5032,7 +5366,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L5" s="35">
         <f>COUNTIF($A$2:$A$80, "*Estudio de Factibilidad*")</f>
@@ -5059,7 +5393,7 @@
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L6" s="35">
         <f>COUNTIF($A$2:$A$80, "*Informe Final de SQA*")</f>
@@ -5086,7 +5420,7 @@
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L7" s="35">
         <f>COUNTIF($A$2:$A$80, "*Modelo de Negocio*")</f>
@@ -5113,7 +5447,7 @@
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Gestión de Configuración*")</f>
@@ -5140,7 +5474,7 @@
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L9" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Iteración*")</f>
@@ -5167,7 +5501,7 @@
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L10" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Proyecto (Ejemplo Gantt)*")</f>
@@ -5194,7 +5528,7 @@
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Proyecto*")</f>
@@ -5221,7 +5555,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L12" s="35">
         <f>COUNTIF($A$2:$A$80, "*Propuesta de Desarrollo*")</f>
@@ -5248,7 +5582,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L13" s="35">
         <f>COUNTIF($A$2:$A$80, "*Resumen de Entrevista*")</f>
@@ -5275,7 +5609,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L14" s="35">
         <f>COUNTIF($A$2:$A$80, "*Resumen de Reunión*")</f>
@@ -5302,7 +5636,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L15" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Calidad*")</f>
@@ -5329,7 +5663,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L16" s="35">
         <f>COUNTIF($A$2:$A$80, "*GitHub*")</f>
@@ -5356,7 +5690,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L17" s="35">
         <f>COUNTIF($A$2:$A$80, "*Herramientas y Tecnologias*")</f>
@@ -5383,7 +5717,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L18" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan Cierre iteracion fase Elaboracion iteracion 1*")</f>
@@ -5410,7 +5744,7 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L19" s="41">
         <f>COUNTIF($A$2:$A$80, "*Prototipo*")</f>

</xml_diff>

<commit_message>
Documentación - Gestión de SQA
Se realiza el informe final de SQA correspondiente a la fase de construcción iteración 1, se actualizan los documentos ChecklistProductoClave de las revisiones, se actualiza el archivo de nomenclaturas de nombres de documentos para la siguiente fase (construcción iteración 2) y se genera el documento de revisión SQA sobre el plan de riesgos y sus artefactos de trabajo asociados.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\03-Construccion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1585EC-719A-402E-A682-B2AC26D2CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DBC83-5911-49BE-93F1-5873F0DAF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -90,7 +90,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -155,7 +155,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -211,7 +211,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -220,7 +220,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -276,7 +276,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -285,7 +285,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -341,7 +341,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -350,7 +350,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -406,7 +406,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -415,7 +415,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -471,7 +471,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Levipichun:</t>
         </r>
@@ -480,7 +480,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Por favor escriba:
@@ -1115,140 +1115,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: No se encontraron errores de ortografía.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nivel de gravedad</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Leve.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ubicación</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Descripción</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: No se encontraron errores de ortografía.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nivel de gravedad</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Leve.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ubicación</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\C106-OSLO - Identificación, Evaluación y análisis de riesgos - Anexo II 27-10-2024.xlsx</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Descripción</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">: Referencia de índice desactualizado.
 </t>
     </r>
@@ -1296,12 +1162,146 @@
       <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: No se encontraron errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Nulo.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\C106-OSLO - Identificación, Evaluación y análisis de riesgos - Anexo II 27-10-2024.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: No se encontraron errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Nulo.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1329,19 +1329,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2568,7 +2555,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations xWindow="600" yWindow="466" count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Responsable" prompt="¿Que integrante del equipo de desarrollo realizo la revisión?" sqref="H2:H20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$66:$A$69</formula1>
@@ -3087,7 +3074,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="7">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F2:F20" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otras opciones de resultado." promptTitle="Estado" prompt="¿Fue resuelto?" sqref="G2:G20" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -4265,7 +4252,7 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4347,7 +4334,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K2" t="s">
         <v>98</v>
@@ -4422,7 +4409,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K4" t="s">
         <v>95</v>
@@ -4720,7 +4707,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations xWindow="732" yWindow="453" count="6">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F2:F20" xr:uid="{00000000-0002-0000-0500-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otras opciones de resultado." promptTitle="Estado" prompt="¿Fue resuelto?" sqref="G2:G20" xr:uid="{00000000-0002-0000-0500-000001000000}">
@@ -6518,7 +6505,7 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="P1:T1"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F2:F28 F31:F63" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C2:C28 C31:C63" xr:uid="{00000000-0002-0000-0700-000003000000}"/>

</xml_diff>

<commit_message>
Documentación - Revisión Técnica Formal
Se realiza la confección del documento correspondiente a la revisión técnica formal al repositorio de GitHub.com.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\03-Construccion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DBC83-5911-49BE-93F1-5873F0DAF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED38293-76CD-493A-899D-3DB0BF2E762E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="115">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1294,6 +1294,76 @@
         <scheme val="minor"/>
       </rPr>
       <t>: Repositorio Testify\Fases_de_desarrollo\03-Construccion\05- Gestion de Proyecto\05- Gestion de Proyecto\C107-OSLO - Seguimiento de Riesgos IIII 27-10-2024.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Revision rutinaria</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en el repositorio, la base de datos de GitHub excede el minimo requerido para trabajar, las consultas de fechas y hashs de commits no responden, exceso de carpetas huerfanas que fueron elimanadas y no desindexadas, los commits pocos descriptivos hacen que el rastreo de los conflictos entre ramas y repositorios locales crezcan en rigor.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Alto.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Repositorio GitHub.com Testify </t>
     </r>
   </si>
 </sst>
@@ -2627,7 +2697,7 @@
       </c>
       <c r="B3" s="28">
         <f>SUM(APOYO!N3,Riesgos!L2,ERS!L2)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -4251,7 +4321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5116,8 +5186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5284,11 +5354,11 @@
       </c>
       <c r="M3" s="32">
         <f>SUM(L3:L80)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="32">
         <f>COUNTIF(A2:A80,"*")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3" s="33">
         <f>COUNTIF($K$3:$K$31, "*")</f>
@@ -5314,16 +5384,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="14"/>
+    <row r="4" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>45593</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>114</v>
+      </c>
       <c r="J4" s="14"/>
       <c r="K4" s="34" t="s">
         <v>69</v>
@@ -5654,7 +5742,7 @@
       </c>
       <c r="L16" s="35">
         <f>COUNTIF($A$2:$A$80, "*GitHub*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="36"/>
       <c r="N16" s="36"/>

</xml_diff>

<commit_message>
Documentación - Gestión SQA
Se revierte el ultimo commit del repositorio rama documentación, se sube por error el software completo a la rama de documentación.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/03-Construccion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\03-Construccion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED38293-76CD-493A-899D-3DB0BF2E762E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D4FB8A-37BE-449B-83BF-C7FDEE887081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="116">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1364,6 +1364,73 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">: Repositorio GitHub.com Testify </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Se sube por error el software completo a la rama de documentación.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify</t>
     </r>
   </si>
 </sst>
@@ -2697,7 +2764,7 @@
       </c>
       <c r="B3" s="28">
         <f>SUM(APOYO!N3,Riesgos!L2,ERS!L2)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -5187,7 +5254,7 @@
   <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5354,11 +5421,11 @@
       </c>
       <c r="M3" s="32">
         <f>SUM(L3:L80)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" s="32">
         <f>COUNTIF(A2:A80,"*")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O3" s="33">
         <f>COUNTIF($K$3:$K$31, "*")</f>
@@ -5429,16 +5496,34 @@
       <c r="S4" s="36"/>
       <c r="T4" s="37"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="13"/>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="12">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F5" s="17">
+        <v>45602</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="J5" s="13"/>
       <c r="K5" s="38" t="s">
         <v>57</v>
@@ -5742,7 +5827,7 @@
       </c>
       <c r="L16" s="35">
         <f>COUNTIF($A$2:$A$80, "*GitHub*")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="36"/>
       <c r="N16" s="36"/>
@@ -6596,7 +6681,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F2:F28 F31:F63" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C2:C28 C31:C63" xr:uid="{00000000-0002-0000-0700-000003000000}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C31:C63 C2:C28" xr:uid="{00000000-0002-0000-0700-000003000000}"/>
     <dataValidation errorStyle="warning" showDropDown="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="E2:E28 E31:E63" xr:uid="{00000000-0002-0000-0700-000005000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Responsable" prompt="¿Que integrante del equipo de desarrollo realizo la revisión?" sqref="H2:H90" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>$A$107:$A$110</formula1>

</xml_diff>